<commit_message>
Continue to add PR feedback
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_report_town_close_prior_year_card_code_5s_comdat.xlsx
+++ b/dbt/export/templates/qc.vw_report_town_close_prior_year_card_code_5s_comdat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Documents\edited_town_close_workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5EA3C6-1F53-494F-890C-827BF0DAA0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FEDDAA-77F2-4FDD-B86C-89A7487000DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F86E03EA-3BEB-4D35-8C8E-3F43C895C1B8}"/>
+    <workbookView xWindow="-33945" yWindow="4005" windowWidth="27765" windowHeight="9525" xr2:uid="{F86E03EA-3BEB-4D35-8C8E-3F43C895C1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB84B27-B683-4D82-A145-2C22439B7F41}">
   <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,7 +554,7 @@
     <col min="24" max="24" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.21875" customWidth="1"/>
     <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10.6640625" bestFit="1" customWidth="1"/>

</xml_diff>